<commit_message>
Manual check of CppDepend and JArchitect results
</commit_message>
<xml_diff>
--- a/results/CoderGears/CppDepend/LICCA/C_Methods_Basics (LICCA).xlsx
+++ b/results/CoderGears/CppDepend/LICCA/C_Methods_Basics (LICCA).xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PREBACIVANJE (D)\UROS - IT\PMF\MASTER\Napredne teme softverskog inženjerstva\Seminarski rad\CoderGears\CppDepend\LICCA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PREBACIVANJE (D)\UROS - IT\PMF\MASTER\Napredne teme softverskog inženjerstva\Seminarski rad\results\CoderGears\CppDepend\LICCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -136,9 +136,6 @@
     <t>}</t>
   </si>
   <si>
-    <t>51 methods</t>
-  </si>
-  <si>
     <t># lines of code (LOC)</t>
   </si>
   <si>
@@ -290,6 +287,9 @@
   </si>
   <si>
     <t>Variance:</t>
+  </si>
+  <si>
+    <t>34 methods</t>
   </si>
 </sst>
 </file>
@@ -866,7 +866,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -900,6 +900,9 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="23" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="23" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1249,8 +1252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -1318,33 +1321,33 @@
     </row>
     <row r="13" spans="1:8" ht="28.8">
       <c r="A13" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="D13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="F13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="G13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="H13" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="7">
         <v>0</v>
@@ -1365,12 +1368,12 @@
         <v>1</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="9">
         <v>9</v>
@@ -1391,12 +1394,12 @@
         <v>0</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="9">
         <v>0</v>
@@ -1417,12 +1420,12 @@
         <v>1</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="7">
         <v>9</v>
@@ -1443,12 +1446,12 @@
         <v>0</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="7">
         <v>0</v>
@@ -1469,12 +1472,12 @@
         <v>1</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" s="9">
         <v>9</v>
@@ -1495,12 +1498,12 @@
         <v>0</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="9">
         <v>0</v>
@@ -1521,12 +1524,12 @@
         <v>1</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="7">
         <v>9</v>
@@ -1547,12 +1550,12 @@
         <v>0</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="7">
         <v>0</v>
@@ -1573,12 +1576,12 @@
         <v>1</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="9">
         <v>9</v>
@@ -1599,12 +1602,12 @@
         <v>0</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B24" s="9">
         <v>0</v>
@@ -1625,12 +1628,12 @@
         <v>1</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B25" s="7">
         <v>9</v>
@@ -1651,12 +1654,12 @@
         <v>0</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B26" s="7">
         <v>0</v>
@@ -1677,12 +1680,12 @@
         <v>1</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B27" s="9">
         <v>9</v>
@@ -1703,12 +1706,12 @@
         <v>0</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B28" s="9">
         <v>0</v>
@@ -1729,12 +1732,12 @@
         <v>1</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B29" s="7">
         <v>9</v>
@@ -1755,38 +1758,38 @@
         <v>0</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="7">
+        <v>0</v>
+      </c>
+      <c r="C30" s="7">
+        <v>0</v>
+      </c>
+      <c r="D30" s="7">
+        <v>1</v>
+      </c>
+      <c r="E30" s="7">
+        <v>0</v>
+      </c>
+      <c r="F30" s="7">
+        <v>0</v>
+      </c>
+      <c r="G30" s="7">
+        <v>1</v>
+      </c>
+      <c r="H30" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="B30" s="7">
-        <v>0</v>
-      </c>
-      <c r="C30" s="7">
-        <v>0</v>
-      </c>
-      <c r="D30" s="7">
-        <v>1</v>
-      </c>
-      <c r="E30" s="7">
-        <v>0</v>
-      </c>
-      <c r="F30" s="7">
-        <v>0</v>
-      </c>
-      <c r="G30" s="7">
-        <v>1</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B31" s="9">
         <v>9</v>
@@ -1807,12 +1810,12 @@
         <v>0</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B32" s="9">
         <v>0</v>
@@ -1833,12 +1836,12 @@
         <v>1</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B33" s="7">
         <v>10</v>
@@ -1859,12 +1862,12 @@
         <v>0</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B34" s="7">
         <v>0</v>
@@ -1885,12 +1888,12 @@
         <v>1</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B35" s="9">
         <v>8</v>
@@ -1911,12 +1914,12 @@
         <v>0</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B36" s="9">
         <v>0</v>
@@ -1937,12 +1940,12 @@
         <v>1</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B37" s="7">
         <v>10</v>
@@ -1963,12 +1966,12 @@
         <v>0</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B38" s="7">
         <v>0</v>
@@ -1989,12 +1992,12 @@
         <v>1</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B39" s="9">
         <v>9</v>
@@ -2015,12 +2018,12 @@
         <v>0</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B40" s="9">
         <v>0</v>
@@ -2041,12 +2044,12 @@
         <v>1</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B41" s="7">
         <v>9</v>
@@ -2067,12 +2070,12 @@
         <v>0</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B42" s="7">
         <v>0</v>
@@ -2093,12 +2096,12 @@
         <v>1</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B43" s="9">
         <v>9</v>
@@ -2119,12 +2122,12 @@
         <v>0</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B44" s="9">
         <v>0</v>
@@ -2145,12 +2148,12 @@
         <v>1</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B45" s="7">
         <v>8</v>
@@ -2171,12 +2174,12 @@
         <v>0</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B46" s="7">
         <v>0</v>
@@ -2197,12 +2200,12 @@
         <v>1</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B47" s="9">
         <v>7</v>
@@ -2223,38 +2226,38 @@
         <v>0</v>
       </c>
       <c r="H47" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="28.8">
       <c r="A48" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B48" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="C48" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="D48" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="E48" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E48" s="5" t="s">
+      <c r="F48" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F48" s="5" t="s">
+      <c r="G48" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G48" s="5" t="s">
+      <c r="H48" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="H48" s="5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B49" s="10">
         <v>151</v>
@@ -2278,7 +2281,7 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B50" s="13">
         <v>4.4411764705882355</v>
@@ -2302,7 +2305,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B51" s="10">
         <v>0</v>
@@ -2326,7 +2329,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B52" s="12">
         <v>10</v>
@@ -2350,7 +2353,7 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B53" s="14">
         <v>4.4668134218174727</v>
@@ -2370,11 +2373,11 @@
       <c r="G53" s="14">
         <v>0.5</v>
       </c>
-      <c r="H53" s="11"/>
+      <c r="H53" s="15"/>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B54" s="13">
         <v>19.952422145328718</v>

</xml_diff>